<commit_message>
Created a trivial sample CSV
</commit_message>
<xml_diff>
--- a/docs/TeamsSimReportSample.xlsx
+++ b/docs/TeamsSimReportSample.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marklevison/Documents/GitHub/high-performance-teams-game/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3A0DD64-E60E-9846-8DE2-20E70336C3DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8829A586-7D81-A045-84F2-5A89B970B483}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8740" yWindow="5000" windowWidth="29800" windowHeight="20280" xr2:uid="{0583A311-9A09-CA4C-87C3-FAD6F4414E1B}"/>
+    <workbookView xWindow="22580" yWindow="3800" windowWidth="29800" windowHeight="20280" xr2:uid="{0583A311-9A09-CA4C-87C3-FAD6F4414E1B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="22">
   <si>
     <t>Game #</t>
   </si>
@@ -61,9 +61,6 @@
   </si>
   <si>
     <t>gremlin</t>
-  </si>
-  <si>
-    <t>Raw Score</t>
   </si>
   <si>
     <t>Final Capacity</t>
@@ -98,6 +95,24 @@
       </rPr>
       <t>I don't think we've ever fixed a limit - how many does the sim choose per round??</t>
     </r>
+  </si>
+  <si>
+    <t>Clarify Product Vision</t>
+  </si>
+  <si>
+    <t>Protected from Outside Distraction</t>
+  </si>
+  <si>
+    <t>All Work is Done on Main or Trunk</t>
+  </si>
+  <si>
+    <t>Unit Testing</t>
+  </si>
+  <si>
+    <t>Remote Team Avatars</t>
+  </si>
+  <si>
+    <t>Poor Quality</t>
   </si>
 </sst>
 </file>
@@ -149,11 +164,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -469,35 +488,35 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7625A3A-6D48-704D-9552-F39C9B8A2C2D}">
-  <dimension ref="A1:V6"/>
+  <dimension ref="A1:V8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" t="s">
         <v>13</v>
-      </c>
-      <c r="B1" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A2" s="1"/>
       <c r="B2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A3" s="1"/>
       <c r="B3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:22" ht="51" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>0</v>
       </c>
@@ -519,31 +538,34 @@
       <c r="O5" t="s">
         <v>7</v>
       </c>
-      <c r="T5" t="s">
+      <c r="T5" s="2" t="s">
         <v>9</v>
       </c>
+      <c r="U5" s="2" t="s">
+        <v>10</v>
+      </c>
       <c r="V5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:22" ht="51" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="C6" t="s">
-        <v>5</v>
-      </c>
-      <c r="D6" t="s">
-        <v>5</v>
+        <v>17</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>17</v>
       </c>
       <c r="E6" t="s">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="F6" t="s">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="G6" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="H6" t="s">
         <v>5</v>
@@ -564,7 +586,7 @@
         <v>5</v>
       </c>
       <c r="O6" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="P6" t="s">
         <v>8</v>
@@ -578,12 +600,18 @@
       <c r="S6" t="s">
         <v>8</v>
       </c>
-      <c r="T6" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="U6" s="2" t="s">
-        <v>11</v>
-      </c>
+      <c r="T6">
+        <v>45</v>
+      </c>
+      <c r="U6">
+        <v>75</v>
+      </c>
+      <c r="V6">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="E8" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>